<commit_message>
improve --container option, add --output-format, etc.
</commit_message>
<xml_diff>
--- a/samples/sample.xlsx
+++ b/samples/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhata\OneDrive\デスクトップ\GIT\xlsx2json\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\xlsx2json\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22604D32-92CC-4E28-9F31-5E8470754E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B304DA86-F376-4D49-B43B-A3B61FC206E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="json.closed" localSheetId="1">Sheet2!$B$1</definedName>
     <definedName name="json.command_test">Sheet1!$K$16</definedName>
-    <definedName name="json.customer.address">Sheet1!$K$8</definedName>
+    <definedName name="json.customer.address">Sheet1!$K$8,Sheet1!$L$8,Sheet1!$M$8</definedName>
     <definedName name="json.customer.name">Sheet1!$K$7</definedName>
     <definedName name="json.datetime">Sheet1!$K$14</definedName>
     <definedName name="json.num">Sheet1!$K$13</definedName>
@@ -32,25 +32,27 @@
     <definedName name="json.v.e.r.y.v.e.r.y.d.e.e.p">Sheet1!$K$18</definedName>
     <definedName name="json.v.e.r.y.v.e.r.y.d.e.e.p.p.a.t.h">Sheet1!$K$17</definedName>
     <definedName name="json.v.e.r.y.v.e.r.y.d.e.e.p.v1">Sheet1!$K$19</definedName>
-    <definedName name="json.ツリー1.lv1.1.A">Sheet1!$K$40</definedName>
-    <definedName name="json.ツリー1.lv1.1.lv2.1.B">Sheet1!$K$42</definedName>
-    <definedName name="json.ツリー1.lv1.1.lv2.1.lv3.1.C">Sheet1!$K$44</definedName>
-    <definedName name="json.ツリー1.lv1.1.lv2.1.lv3.1.seq">Sheet1!$K$43</definedName>
-    <definedName name="json.ツリー1.lv1.1.lv2.1.seq">Sheet1!$K$41</definedName>
-    <definedName name="json.ツリー1.lv1.1.seq">Sheet1!$K$39</definedName>
-    <definedName name="json.リスト1.aaaコード.1">Sheet1!$N$31</definedName>
-    <definedName name="json.リスト1.aaa名称.1">Sheet1!$K$31</definedName>
-    <definedName name="json.リスト1.bbbコード.1">Sheet1!$N$34</definedName>
-    <definedName name="json.リスト1.bbb名称.1">Sheet1!$K$34</definedName>
+    <definedName name="json.ツリー1.lv1.1">Sheet1!$A$40:$Q$49</definedName>
+    <definedName name="json.ツリー1.lv1.1.A">Sheet1!$K$41</definedName>
+    <definedName name="json.ツリー1.lv1.1.lv2.1">Sheet1!$B$42:$Q$47</definedName>
+    <definedName name="json.ツリー1.lv1.1.lv2.1.B">Sheet1!$K$43</definedName>
+    <definedName name="json.ツリー1.lv1.1.lv2.1.lv3.1">Sheet1!$C$44:$Q$45</definedName>
+    <definedName name="json.ツリー1.lv1.1.lv2.1.lv3.1.C">Sheet1!$K$45</definedName>
+    <definedName name="json.ツリー1.lv1.1.lv2.1.lv3.1.seq">Sheet1!$K$44</definedName>
+    <definedName name="json.ツリー1.lv1.1.lv2.1.seq">Sheet1!$K$42</definedName>
+    <definedName name="json.ツリー1.lv1.1.seq">Sheet1!$K$40</definedName>
+    <definedName name="json.リスト1.1">Sheet1!$A$31:$Q$33</definedName>
+    <definedName name="json.リスト1.1.1">Sheet1!$K$31:$Q$31</definedName>
+    <definedName name="json.リスト1.1.1.aaaコード">Sheet1!$N$31:$Q$31</definedName>
+    <definedName name="json.リスト1.1.1.aaa名称">Sheet1!$K$31</definedName>
     <definedName name="json.日本語_._記_号__">Sheet1!$K$11</definedName>
     <definedName name="json.日本語_.記号_">Sheet1!$K$10</definedName>
-    <definedName name="json.表1.列A.1">Sheet1!$A$26</definedName>
-    <definedName name="json.表1.列B.1">Sheet1!$K$26</definedName>
-    <definedName name="json.表1.列C.1">Sheet1!$N$26</definedName>
+    <definedName name="json.表1">Sheet1!$A$26:$Q$27</definedName>
+    <definedName name="json.表1.1">Sheet1!$A$26:$Q$26</definedName>
+    <definedName name="json.表1.1.列A">Sheet1!$A$26</definedName>
+    <definedName name="json.表1.1.列B">Sheet1!$K$26</definedName>
+    <definedName name="json.表1.1.列C">Sheet1!$N$26</definedName>
     <definedName name="otherprefix.test">Sheet1!$K$22</definedName>
-    <definedName name="ツリー1.range">Sheet1!$A$39:$Q$54</definedName>
-    <definedName name="リスト1.range">Sheet1!$A$31:$Q$36</definedName>
-    <definedName name="表1.range">Sheet1!$A$25:$Q$28</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>parent</t>
     <phoneticPr fontId="1"/>
@@ -72,13 +74,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>山田太郎</t>
-    <rPh sb="0" eb="4">
-      <t>ヤマダタロウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>G2</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -95,10 +90,6 @@
   </si>
   <si>
     <t>address</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>とうきょう</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -234,76 +225,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>bbb名称|bbbコード</t>
-    <rPh sb="3" eb="5">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>aaa名称1</t>
-    <rPh sb="3" eb="5">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>aaa名称2</t>
-    <rPh sb="3" eb="5">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>aaa名称3</t>
-    <rPh sb="3" eb="5">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bbb名称1</t>
-    <rPh sb="3" eb="5">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bbb名称2</t>
-    <rPh sb="3" eb="5">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bbb名称3</t>
-    <rPh sb="3" eb="5">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>aaaコード11,aaaコード12</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>aaaコード21,aaaコード22</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>aaaコード31,aaaコード32</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bbbコード11,bbbコード12</t>
-  </si>
-  <si>
-    <t>bbbコード21,bbbコード22</t>
-  </si>
-  <si>
-    <t>bbbコード31,bbbコード32</t>
-  </si>
-  <si>
     <t>A1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -437,6 +358,124 @@
   </si>
   <si>
     <t>ツリー1</t>
+  </si>
+  <si>
+    <t>aaa名称11</t>
+    <rPh sb="3" eb="5">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa名称12</t>
+    <rPh sb="3" eb="5">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa名称13</t>
+    <rPh sb="3" eb="5">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa名称21</t>
+    <rPh sb="3" eb="5">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa名称22</t>
+    <rPh sb="3" eb="5">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa名称31</t>
+    <rPh sb="3" eb="5">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa11-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa11-2</t>
+  </si>
+  <si>
+    <t>aaa12-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa12-2</t>
+  </si>
+  <si>
+    <t>aaa13-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa21-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa21-2</t>
+  </si>
+  <si>
+    <t>aaa22-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa31-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa11-3</t>
+  </si>
+  <si>
+    <t>aaa名称41</t>
+    <rPh sb="3" eb="5">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa41-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa名称|aaaコードX</t>
+    <rPh sb="3" eb="5">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>かつしかく</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>しばまた</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>とうきょうと</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>山田 太郎</t>
+    <rPh sb="0" eb="2">
+      <t>ヤマダ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>タロウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -935,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q54"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="114" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -948,167 +987,173 @@
     <col min="15" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="36">
+    <row r="2" spans="1:13" ht="36">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="36">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
+      <c r="K7" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="B8" s="1" t="s">
+      <c r="K8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K13" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K14" s="3">
         <f ca="1">TODAY()</f>
-        <v>45860</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>45906</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K15" s="5">
         <v>0.52425925925925931</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="54">
+    <row r="16" spans="1:13" ht="54">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="17.399999999999999" customHeight="1"/>
     <row r="21" spans="1:17">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="14" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -1120,12 +1165,12 @@
       <c r="I25" s="15"/>
       <c r="J25" s="16"/>
       <c r="K25" s="14" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="L25" s="15"/>
       <c r="M25" s="16"/>
       <c r="N25" s="14" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
@@ -1133,7 +1178,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="14" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1145,12 +1190,12 @@
       <c r="I26" s="15"/>
       <c r="J26" s="16"/>
       <c r="K26" s="14" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="L26" s="15"/>
       <c r="M26" s="16"/>
       <c r="N26" s="14" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
@@ -1158,7 +1203,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="14" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1170,12 +1215,12 @@
       <c r="I27" s="15"/>
       <c r="J27" s="16"/>
       <c r="K27" s="14" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="L27" s="15"/>
       <c r="M27" s="16"/>
       <c r="N27" s="14" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
@@ -1183,7 +1228,7 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="14" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1195,12 +1240,12 @@
       <c r="I28" s="15"/>
       <c r="J28" s="16"/>
       <c r="K28" s="14" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="L28" s="15"/>
       <c r="M28" s="16"/>
       <c r="N28" s="14" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
@@ -1208,12 +1253,12 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1223,31 +1268,39 @@
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="8"/>
+      <c r="J31" s="8">
+        <v>1</v>
+      </c>
       <c r="K31" s="14" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L31" s="15"/>
       <c r="M31" s="16"/>
       <c r="N31" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
+        <v>76</v>
+      </c>
+      <c r="O31" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="P31" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="Q31" s="16"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="9"/>
       <c r="J32" s="10"/>
       <c r="K32" s="14" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="L32" s="15"/>
       <c r="M32" s="16"/>
       <c r="N32" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O32" s="15"/>
+        <v>78</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="P32" s="15"/>
       <c r="Q32" s="16"/>
     </row>
@@ -1263,12 +1316,12 @@
       <c r="I33" s="12"/>
       <c r="J33" s="13"/>
       <c r="K33" s="14" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="L33" s="15"/>
       <c r="M33" s="16"/>
       <c r="N33" s="14" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
@@ -1276,38 +1329,52 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J34" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="J34" s="10">
+        <v>2</v>
+      </c>
       <c r="K34" s="14" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="L34" s="15"/>
       <c r="M34" s="16"/>
       <c r="N34" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="O34" s="15"/>
+        <v>81</v>
+      </c>
+      <c r="O34" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="P34" s="15"/>
       <c r="Q34" s="16"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="9"/>
-      <c r="J35" s="10"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="13"/>
       <c r="K35" s="14" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="L35" s="15"/>
       <c r="M35" s="16"/>
       <c r="N35" s="14" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="16"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="11"/>
+      <c r="A36" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -1316,52 +1383,58 @@
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
-      <c r="J36" s="13"/>
+      <c r="J36" s="13">
+        <v>3</v>
+      </c>
       <c r="K36" s="14" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="L36" s="15"/>
       <c r="M36" s="16"/>
       <c r="N36" s="14" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="O36" s="15"/>
       <c r="P36" s="15"/>
       <c r="Q36" s="16"/>
     </row>
-    <row r="38" spans="1:17">
-      <c r="A38" s="1" t="s">
-        <v>84</v>
-      </c>
+    <row r="37" spans="1:17">
+      <c r="A37" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="13">
+        <v>4</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="L37" s="15"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="16"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="17" t="s">
+      <c r="A39" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="8"/>
     </row>
     <row r="40" spans="1:17">
-      <c r="A40" s="9"/>
-      <c r="B40" s="14" t="s">
-        <v>66</v>
-      </c>
+      <c r="A40" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
@@ -1370,8 +1443,8 @@
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="15" t="s">
-        <v>51</v>
+      <c r="K40" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
@@ -1382,8 +1455,8 @@
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="9"/>
-      <c r="B41" s="6" t="s">
-        <v>36</v>
+      <c r="B41" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -1393,8 +1466,8 @@
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
       <c r="J41" s="8"/>
-      <c r="K41" s="18" t="s">
-        <v>70</v>
+      <c r="K41" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="L41" s="7"/>
       <c r="M41" s="7"/>
@@ -1405,193 +1478,193 @@
     </row>
     <row r="42" spans="1:17">
       <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="16"/>
+      <c r="B42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="8"/>
     </row>
     <row r="43" spans="1:17">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
-      <c r="C43" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="8"/>
+      <c r="C43" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="16"/>
     </row>
     <row r="44" spans="1:17">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="16"/>
+      <c r="C44" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="8"/>
     </row>
     <row r="45" spans="1:17">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
-      <c r="C45" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="7"/>
-      <c r="Q45" s="8"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="16"/>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="16"/>
-      <c r="K46" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="16"/>
+      <c r="C46" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="8"/>
     </row>
     <row r="47" spans="1:17">
       <c r="A47" s="9"/>
-      <c r="B47" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7"/>
-      <c r="P47" s="7"/>
-      <c r="Q47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="16"/>
     </row>
     <row r="48" spans="1:17">
       <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="14" t="s">
+      <c r="B48" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="8"/>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="16"/>
-    </row>
-    <row r="49" spans="1:17">
-      <c r="A49" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7"/>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="8"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="16"/>
     </row>
     <row r="50" spans="1:17">
-      <c r="A50" s="9"/>
-      <c r="B50" s="14" t="s">
-        <v>66</v>
-      </c>
+      <c r="A50" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
@@ -1600,8 +1673,8 @@
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="15" t="s">
-        <v>74</v>
+      <c r="K50" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
@@ -1612,95 +1685,118 @@
     </row>
     <row r="51" spans="1:17">
       <c r="A51" s="9"/>
-      <c r="B51" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="8"/>
+      <c r="B51" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="16"/>
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="16"/>
-      <c r="K52" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="16"/>
+      <c r="B52" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="8"/>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="9"/>
       <c r="B53" s="9"/>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="16"/>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="8"/>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
-      <c r="P53" s="7"/>
-      <c r="Q53" s="8"/>
-    </row>
-    <row r="54" spans="1:17">
-      <c r="A54" s="11"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="16"/>
-      <c r="K54" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="16"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1713,26 +1809,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B65A99-14ED-4197-AB82-DC4CBE6267BB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>